<commit_message>
Actualizacion de matriz de rastreabilidad
</commit_message>
<xml_diff>
--- a/Proyectos/Activos/Viaticos_q/1. Requerimientos/Viaticos_q_MatrizdeRastreabilidad.xlsx
+++ b/Proyectos/Activos/Viaticos_q/1. Requerimientos/Viaticos_q_MatrizdeRastreabilidad.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\IWM\Repositorio IWM\Proyectos\Activos\Viaticos_q\Requerimientos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\Documents\cabina_press\Proyectos\Activos\Viaticos_q\1. Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
   <si>
     <t>Matriz de trazabilidad</t>
   </si>
@@ -210,6 +210,15 @@
   </si>
   <si>
     <t>Por naturaleza de requerimiento no cuenta con caso de uso</t>
+  </si>
+  <si>
+    <t>3.2.3.4</t>
+  </si>
+  <si>
+    <t>Edicion Gastos y Viaticos</t>
+  </si>
+  <si>
+    <t>CU06</t>
   </si>
 </sst>
 </file>
@@ -483,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -551,6 +560,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -560,15 +584,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -620,6 +635,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -931,13 +947,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN54"/>
+  <dimension ref="A1:AO55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="6" topLeftCell="G17" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="O1" sqref="O1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,16 +962,16 @@
     <col min="2" max="2" width="39.28515625" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="42.42578125" customWidth="1"/>
     <col min="4" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="12" width="5.42578125" customWidth="1"/>
-    <col min="13" max="13" width="37.5703125" customWidth="1"/>
-    <col min="14" max="16" width="5.42578125" customWidth="1"/>
-    <col min="17" max="33" width="5.28515625" customWidth="1"/>
-    <col min="34" max="34" width="14.140625" customWidth="1"/>
-    <col min="35" max="35" width="17.28515625" customWidth="1"/>
-    <col min="36" max="42" width="6.5703125" customWidth="1"/>
+    <col min="8" max="13" width="5.42578125" customWidth="1"/>
+    <col min="14" max="14" width="37.5703125" customWidth="1"/>
+    <col min="15" max="17" width="5.42578125" customWidth="1"/>
+    <col min="18" max="34" width="5.28515625" customWidth="1"/>
+    <col min="35" max="35" width="14.140625" customWidth="1"/>
+    <col min="36" max="36" width="17.28515625" customWidth="1"/>
+    <col min="37" max="43" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -974,17 +990,18 @@
         <v>8</v>
       </c>
       <c r="L1" s="6"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="15"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="19"/>
       <c r="O1" s="15"/>
       <c r="P1" s="15"/>
       <c r="Q1" s="15"/>
-      <c r="R1" s="12"/>
+      <c r="R1" s="15"/>
       <c r="S1" s="12"/>
       <c r="T1" s="12"/>
       <c r="U1" s="12"/>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="V1" s="12"/>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -999,23 +1016,24 @@
         <v>9</v>
       </c>
       <c r="L2" s="8"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="15"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="19"/>
       <c r="O2" s="15"/>
       <c r="P2" s="15"/>
       <c r="Q2" s="15"/>
-      <c r="R2" s="12"/>
+      <c r="R2" s="15"/>
       <c r="S2" s="12"/>
       <c r="T2" s="12"/>
       <c r="U2" s="12"/>
-    </row>
-    <row r="3" spans="1:40" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="V2" s="12"/>
+    </row>
+    <row r="3" spans="1:41" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="45"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="47"/>
       <c r="E3" s="9"/>
       <c r="F3" s="10" t="s">
         <v>12</v>
@@ -1023,35 +1041,36 @@
       <c r="G3" s="11"/>
       <c r="H3" s="18"/>
       <c r="I3" s="16"/>
-      <c r="J3" s="59" t="s">
+      <c r="J3" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="23" t="s">
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="22"/>
       <c r="O3" s="22"/>
       <c r="P3" s="22"/>
       <c r="Q3" s="22"/>
-      <c r="R3" s="12"/>
+      <c r="R3" s="22"/>
       <c r="S3" s="12"/>
       <c r="T3" s="12"/>
       <c r="U3" s="12"/>
-    </row>
-    <row r="4" spans="1:40" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="52" t="s">
+      <c r="V3" s="12"/>
+    </row>
+    <row r="4" spans="1:41" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="48"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="55" t="s">
+      <c r="F4" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="52" t="s">
+      <c r="G4" s="54" t="s">
         <v>15</v>
       </c>
       <c r="H4" s="16"/>
@@ -1060,43 +1079,45 @@
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
-      <c r="N4" s="16"/>
+      <c r="N4" s="17"/>
       <c r="O4" s="16"/>
       <c r="P4" s="16"/>
       <c r="Q4" s="16"/>
-      <c r="R4" s="12"/>
+      <c r="R4" s="16"/>
       <c r="S4" s="12"/>
       <c r="T4" s="12"/>
       <c r="U4" s="12"/>
-    </row>
-    <row r="5" spans="1:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="49"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="58" t="s">
+      <c r="V4" s="12"/>
+    </row>
+    <row r="5" spans="1:41" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="51"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="24" t="s">
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="N5" s="14"/>
       <c r="O5" s="14"/>
       <c r="P5" s="14"/>
       <c r="Q5" s="14"/>
-      <c r="R5" s="13"/>
+      <c r="R5" s="14"/>
       <c r="S5" s="13"/>
       <c r="T5" s="13"/>
       <c r="U5" s="13"/>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="V5" s="13"/>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>2</v>
       </c>
@@ -1109,9 +1130,9 @@
       <c r="D6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="54"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="54"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="56"/>
       <c r="H6" s="8" t="s">
         <v>1</v>
       </c>
@@ -1127,8 +1148,10 @@
       <c r="L6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="25"/>
-      <c r="N6" s="13"/>
+      <c r="M6" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="N6" s="25"/>
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
@@ -1136,7 +1159,7 @@
       <c r="S6" s="13"/>
       <c r="T6" s="13"/>
       <c r="U6" s="13"/>
-      <c r="V6" s="4"/>
+      <c r="V6" s="13"/>
       <c r="W6" s="4"/>
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
@@ -1145,7 +1168,7 @@
       <c r="AB6" s="4"/>
       <c r="AC6" s="4"/>
       <c r="AD6" s="4"/>
-      <c r="AE6" s="5"/>
+      <c r="AE6" s="4"/>
       <c r="AF6" s="5"/>
       <c r="AG6" s="5"/>
       <c r="AH6" s="5"/>
@@ -1155,26 +1178,27 @@
       <c r="AL6" s="5"/>
       <c r="AM6" s="5"/>
       <c r="AN6" s="5"/>
-    </row>
-    <row r="7" spans="1:40" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="AO6" s="5"/>
+    </row>
+    <row r="7" spans="1:41" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="26"/>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="13"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="41"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
@@ -1182,26 +1206,27 @@
       <c r="S7" s="13"/>
       <c r="T7" s="13"/>
       <c r="U7" s="13"/>
-    </row>
-    <row r="8" spans="1:40" ht="18" x14ac:dyDescent="0.25">
+      <c r="V7" s="13"/>
+    </row>
+    <row r="8" spans="1:41" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="28"/>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="13"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="44"/>
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
@@ -1209,8 +1234,9 @@
       <c r="S8" s="13"/>
       <c r="T8" s="13"/>
       <c r="U8" s="13"/>
-    </row>
-    <row r="9" spans="1:40" ht="30" x14ac:dyDescent="0.25">
+      <c r="V8" s="13"/>
+    </row>
+    <row r="9" spans="1:41" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>26</v>
       </c>
@@ -1229,10 +1255,10 @@
       <c r="J9" s="31"/>
       <c r="K9" s="31"/>
       <c r="L9" s="31"/>
-      <c r="M9" s="35" t="s">
+      <c r="M9" s="31"/>
+      <c r="N9" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="N9" s="13"/>
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
@@ -1240,26 +1266,27 @@
       <c r="S9" s="13"/>
       <c r="T9" s="13"/>
       <c r="U9" s="13"/>
-    </row>
-    <row r="10" spans="1:40" ht="18" x14ac:dyDescent="0.25">
+      <c r="V9" s="13"/>
+    </row>
+    <row r="10" spans="1:41" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="28"/>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="13"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="44"/>
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
@@ -1267,8 +1294,9 @@
       <c r="S10" s="13"/>
       <c r="T10" s="13"/>
       <c r="U10" s="13"/>
-    </row>
-    <row r="11" spans="1:40" ht="30" x14ac:dyDescent="0.25">
+      <c r="V10" s="13"/>
+    </row>
+    <row r="11" spans="1:41" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
         <v>31</v>
       </c>
@@ -1287,10 +1315,10 @@
       <c r="J11" s="34"/>
       <c r="K11" s="34"/>
       <c r="L11" s="34"/>
-      <c r="M11" s="35" t="s">
+      <c r="M11" s="34"/>
+      <c r="N11" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="N11" s="13"/>
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
@@ -1298,8 +1326,9 @@
       <c r="S11" s="13"/>
       <c r="T11" s="13"/>
       <c r="U11" s="13"/>
-    </row>
-    <row r="12" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V11" s="13"/>
+    </row>
+    <row r="12" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="32"/>
       <c r="B12" s="32"/>
       <c r="C12" s="32"/>
@@ -1314,8 +1343,8 @@
       <c r="J12" s="34"/>
       <c r="K12" s="34"/>
       <c r="L12" s="34"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="13"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="27"/>
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
@@ -1323,8 +1352,9 @@
       <c r="S12" s="13"/>
       <c r="T12" s="13"/>
       <c r="U12" s="13"/>
-    </row>
-    <row r="13" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V12" s="13"/>
+    </row>
+    <row r="13" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="32"/>
       <c r="B13" s="32"/>
       <c r="C13" s="32"/>
@@ -1339,8 +1369,8 @@
       <c r="J13" s="34"/>
       <c r="K13" s="34"/>
       <c r="L13" s="34"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="13"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="27"/>
       <c r="O13" s="13"/>
       <c r="P13" s="13"/>
       <c r="Q13" s="13"/>
@@ -1348,8 +1378,9 @@
       <c r="S13" s="13"/>
       <c r="T13" s="13"/>
       <c r="U13" s="13"/>
-    </row>
-    <row r="14" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V13" s="13"/>
+    </row>
+    <row r="14" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="32"/>
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
@@ -1364,8 +1395,8 @@
       <c r="J14" s="34"/>
       <c r="K14" s="34"/>
       <c r="L14" s="34"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="13"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="27"/>
       <c r="O14" s="13"/>
       <c r="P14" s="13"/>
       <c r="Q14" s="13"/>
@@ -1373,26 +1404,27 @@
       <c r="S14" s="13"/>
       <c r="T14" s="13"/>
       <c r="U14" s="13"/>
-    </row>
-    <row r="15" spans="1:40" ht="18" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="V14" s="13"/>
+    </row>
+    <row r="15" spans="1:41" ht="18" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="28"/>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="13"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="44"/>
       <c r="O15" s="13"/>
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
@@ -1400,8 +1432,9 @@
       <c r="S15" s="13"/>
       <c r="T15" s="13"/>
       <c r="U15" s="13"/>
-    </row>
-    <row r="16" spans="1:40" ht="30" x14ac:dyDescent="0.25">
+      <c r="V15" s="13"/>
+    </row>
+    <row r="16" spans="1:41" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
         <v>35</v>
       </c>
@@ -1420,10 +1453,10 @@
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
       <c r="L16" s="34"/>
-      <c r="M16" s="35" t="s">
+      <c r="M16" s="34"/>
+      <c r="N16" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="N16" s="13"/>
       <c r="O16" s="13"/>
       <c r="P16" s="13"/>
       <c r="Q16" s="13"/>
@@ -1431,26 +1464,27 @@
       <c r="S16" s="13"/>
       <c r="T16" s="13"/>
       <c r="U16" s="13"/>
-    </row>
-    <row r="17" spans="1:31" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="V16" s="13"/>
+    </row>
+    <row r="17" spans="1:32" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="26"/>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="13"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="41"/>
       <c r="O17" s="13"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="13"/>
@@ -1458,8 +1492,9 @@
       <c r="S17" s="13"/>
       <c r="T17" s="13"/>
       <c r="U17" s="13"/>
-    </row>
-    <row r="18" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="V17" s="13"/>
+    </row>
+    <row r="18" spans="1:32" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
         <v>28</v>
       </c>
@@ -1478,10 +1513,10 @@
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
       <c r="L18" s="32"/>
-      <c r="M18" s="35" t="s">
+      <c r="M18" s="32"/>
+      <c r="N18" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="N18" s="13"/>
       <c r="O18" s="13"/>
       <c r="P18" s="13"/>
       <c r="Q18" s="13"/>
@@ -1489,8 +1524,9 @@
       <c r="S18" s="13"/>
       <c r="T18" s="13"/>
       <c r="U18" s="13"/>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="V18" s="13"/>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
         <v>39</v>
       </c>
@@ -1511,8 +1547,8 @@
       <c r="J19" s="32"/>
       <c r="K19" s="32"/>
       <c r="L19" s="32"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="13"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="27"/>
       <c r="O19" s="13"/>
       <c r="P19" s="13"/>
       <c r="Q19" s="13"/>
@@ -1520,26 +1556,27 @@
       <c r="S19" s="13"/>
       <c r="T19" s="13"/>
       <c r="U19" s="13"/>
-    </row>
-    <row r="20" spans="1:31" ht="18" x14ac:dyDescent="0.25">
+      <c r="V19" s="13"/>
+    </row>
+    <row r="20" spans="1:32" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
         <v>40</v>
       </c>
       <c r="B20" s="32"/>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="13"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="44"/>
       <c r="O20" s="13"/>
       <c r="P20" s="13"/>
       <c r="Q20" s="13"/>
@@ -1547,8 +1584,9 @@
       <c r="S20" s="13"/>
       <c r="T20" s="13"/>
       <c r="U20" s="13"/>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="V20" s="13"/>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
         <v>42</v>
       </c>
@@ -1569,8 +1607,8 @@
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
       <c r="L21" s="32"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="13"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="27"/>
       <c r="O21" s="13"/>
       <c r="P21" s="13"/>
       <c r="Q21" s="13"/>
@@ -1578,8 +1616,9 @@
       <c r="S21" s="13"/>
       <c r="T21" s="13"/>
       <c r="U21" s="13"/>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="V21" s="13"/>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
         <v>45</v>
       </c>
@@ -1600,8 +1639,8 @@
       </c>
       <c r="K22" s="32"/>
       <c r="L22" s="32"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="13"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="27"/>
       <c r="O22" s="13"/>
       <c r="P22" s="13"/>
       <c r="Q22" s="13"/>
@@ -1609,8 +1648,9 @@
       <c r="S22" s="13"/>
       <c r="T22" s="13"/>
       <c r="U22" s="13"/>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="V22" s="13"/>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
         <v>46</v>
       </c>
@@ -1631,8 +1671,8 @@
         <v>59</v>
       </c>
       <c r="L23" s="32"/>
-      <c r="M23" s="27"/>
-      <c r="N23" s="13"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="27"/>
       <c r="O23" s="13"/>
       <c r="P23" s="13"/>
       <c r="Q23" s="13"/>
@@ -1640,14 +1680,15 @@
       <c r="S23" s="13"/>
       <c r="T23" s="13"/>
       <c r="U23" s="13"/>
-    </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="V23" s="13"/>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B24" s="32"/>
-      <c r="C24" s="33" t="s">
-        <v>48</v>
+      <c r="C24" t="s">
+        <v>62</v>
       </c>
       <c r="D24" s="32" t="s">
         <v>10</v>
@@ -1659,11 +1700,11 @@
       <c r="I24" s="32"/>
       <c r="J24" s="32"/>
       <c r="K24" s="32"/>
-      <c r="L24" s="32" t="s">
+      <c r="L24" s="32"/>
+      <c r="M24" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="M24" s="27"/>
-      <c r="N24" s="13"/>
+      <c r="N24" s="27"/>
       <c r="O24" s="13"/>
       <c r="P24" s="13"/>
       <c r="Q24" s="13"/>
@@ -1671,26 +1712,31 @@
       <c r="S24" s="13"/>
       <c r="T24" s="13"/>
       <c r="U24" s="13"/>
-    </row>
-    <row r="25" spans="1:31" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
-        <v>57</v>
+      <c r="V24" s="13"/>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A25" s="32" t="s">
+        <v>49</v>
       </c>
       <c r="B25" s="32"/>
-      <c r="C25" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="42"/>
-      <c r="N25" s="13"/>
+      <c r="C25" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="M25" s="32"/>
+      <c r="N25" s="27"/>
       <c r="O25" s="13"/>
       <c r="P25" s="13"/>
       <c r="Q25" s="13"/>
@@ -1698,30 +1744,27 @@
       <c r="S25" s="13"/>
       <c r="T25" s="13"/>
       <c r="U25" s="13"/>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
-        <v>51</v>
+      <c r="V25" s="13"/>
+    </row>
+    <row r="26" spans="1:32" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="B26" s="32"/>
-      <c r="C26" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="27"/>
-      <c r="N26" s="13"/>
+      <c r="C26" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="40"/>
+      <c r="N26" s="41"/>
       <c r="O26" s="13"/>
       <c r="P26" s="13"/>
       <c r="Q26" s="13"/>
@@ -1729,14 +1772,15 @@
       <c r="S26" s="13"/>
       <c r="T26" s="13"/>
       <c r="U26" s="13"/>
-    </row>
-    <row r="27" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="V26" s="13"/>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" s="32"/>
       <c r="C27" s="33" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D27" s="32" t="s">
         <v>10</v>
@@ -1744,15 +1788,15 @@
       <c r="E27" s="32"/>
       <c r="F27" s="32"/>
       <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
+      <c r="H27" s="32" t="s">
+        <v>59</v>
+      </c>
       <c r="I27" s="32"/>
       <c r="J27" s="32"/>
       <c r="K27" s="32"/>
       <c r="L27" s="32"/>
-      <c r="M27" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="N27" s="13"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="27"/>
       <c r="O27" s="13"/>
       <c r="P27" s="13"/>
       <c r="Q27" s="13"/>
@@ -1760,14 +1804,15 @@
       <c r="S27" s="13"/>
       <c r="T27" s="13"/>
       <c r="U27" s="13"/>
-    </row>
-    <row r="28" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="V27" s="13"/>
+    </row>
+    <row r="28" spans="1:32" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="32" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B28" s="32"/>
       <c r="C28" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D28" s="32" t="s">
         <v>10</v>
@@ -1775,15 +1820,15 @@
       <c r="E28" s="32"/>
       <c r="F28" s="32"/>
       <c r="G28" s="32"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="35" t="s">
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="N28" s="13"/>
       <c r="O28" s="13"/>
       <c r="P28" s="13"/>
       <c r="Q28" s="13"/>
@@ -1791,36 +1836,41 @@
       <c r="S28" s="13"/>
       <c r="T28" s="13"/>
       <c r="U28" s="13"/>
-    </row>
-    <row r="29" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="W29" s="1"/>
-      <c r="X29" s="1"/>
-      <c r="Y29" s="1"/>
-      <c r="Z29" s="1"/>
-      <c r="AA29" s="1"/>
-      <c r="AB29" s="1"/>
-      <c r="AC29" s="1"/>
-      <c r="AD29" s="1"/>
-      <c r="AE29" s="1"/>
-    </row>
-    <row r="30" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V28" s="13"/>
+    </row>
+    <row r="29" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="32"/>
+      <c r="C29" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="34"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="34"/>
+      <c r="N29" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="13"/>
+      <c r="U29" s="13"/>
+      <c r="V29" s="13"/>
+    </row>
+    <row r="30" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1833,8 +1883,23 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
-    </row>
-    <row r="31" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M30" s="62"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="1"/>
+      <c r="AD30" s="1"/>
+      <c r="AE30" s="1"/>
+      <c r="AF30" s="1"/>
+    </row>
+    <row r="31" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1847,8 +1912,9 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
-    </row>
-    <row r="32" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M31" s="62"/>
+    </row>
+    <row r="32" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1861,8 +1927,9 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
-    </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M32" s="62"/>
+    </row>
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1875,8 +1942,9 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
-    </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M33" s="62"/>
+    </row>
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1889,45 +1957,61 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
-    </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="M34" s="62"/>
+    </row>
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="62"/>
+    </row>
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="49" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="50" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="51" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="52" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="53" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="54" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C25:M25"/>
-    <mergeCell ref="C10:M10"/>
+    <mergeCell ref="C26:N26"/>
+    <mergeCell ref="C10:N10"/>
     <mergeCell ref="A3:D5"/>
     <mergeCell ref="E4:E6"/>
     <mergeCell ref="F4:F6"/>
     <mergeCell ref="G4:G6"/>
     <mergeCell ref="H5:L5"/>
     <mergeCell ref="J3:L3"/>
-    <mergeCell ref="C8:M8"/>
-    <mergeCell ref="C7:M7"/>
-    <mergeCell ref="C15:M15"/>
-    <mergeCell ref="C17:M17"/>
-    <mergeCell ref="C20:M20"/>
+    <mergeCell ref="C8:N8"/>
+    <mergeCell ref="C7:N7"/>
+    <mergeCell ref="C15:N15"/>
+    <mergeCell ref="C17:N17"/>
+    <mergeCell ref="C20:N20"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:G14 D16:G16 D26:G34 D18:G19 D21:G24 D9:G9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:G14 D16:G16 D27:G35 D18:G19 D21:G25 D9:G9">
       <formula1>"Activo,Concluido,Eliminado,M-Activo,M-Concluido,M-Eliminado"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>